<commit_message>
VCU Build, start code
</commit_message>
<xml_diff>
--- a/VehicleController/VehicleController.xlsx
+++ b/VehicleController/VehicleController.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\GitHub\UNCAMotorsports-2017\VehicleController\"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="176">
   <si>
     <t>Reference</t>
   </si>
@@ -1410,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,6 +2184,9 @@
       <c r="D45" t="s">
         <v>12</v>
       </c>
+      <c r="E45" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -2226,6 +2229,9 @@
       <c r="D48" t="s">
         <v>91</v>
       </c>
+      <c r="E48" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -2240,6 +2246,9 @@
       <c r="D49" t="s">
         <v>72</v>
       </c>
+      <c r="E49" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -2254,6 +2263,9 @@
       <c r="D50" t="s">
         <v>72</v>
       </c>
+      <c r="E50" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -2268,6 +2280,9 @@
       <c r="D51" t="s">
         <v>72</v>
       </c>
+      <c r="E51" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -2282,6 +2297,9 @@
       <c r="D52" t="s">
         <v>72</v>
       </c>
+      <c r="E52" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -2296,6 +2314,9 @@
       <c r="D53" t="s">
         <v>72</v>
       </c>
+      <c r="E53" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -2395,6 +2416,9 @@
       <c r="D59" t="s">
         <v>101</v>
       </c>
+      <c r="E59" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -2426,6 +2450,9 @@
       <c r="D61" t="s">
         <v>101</v>
       </c>
+      <c r="E61" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -2457,6 +2484,9 @@
       <c r="D63" t="s">
         <v>101</v>
       </c>
+      <c r="E63" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2539,6 +2569,9 @@
       <c r="D68" t="s">
         <v>96</v>
       </c>
+      <c r="E68" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -2567,6 +2600,9 @@
       <c r="D70" t="s">
         <v>132</v>
       </c>
+      <c r="E70" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -2580,6 +2616,9 @@
       </c>
       <c r="D71" t="s">
         <v>166</v>
+      </c>
+      <c r="E71" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>